<commit_message>
Fixed all application to prepare it to be easier to add a new viscoelastic model or a new operation.
</commit_message>
<xml_diff>
--- a/sheets/númerosvisco.xlsx
+++ b/sheets/númerosvisco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\IC Tecidos Moles\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1769E5F8-727B-4B6E-9A1F-864890861694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBC80F2-21EB-4DEB-8A7B-57582F4DDA44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
+    <workbookView xWindow="4800" yWindow="4560" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
     <t>ACL - porco</t>
   </si>
@@ -188,23 +188,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">197,38 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 15,53</t>
-    </r>
-  </si>
-  <si>
-    <t>A (Mpa)</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">0,632 </t>
     </r>
     <r>
@@ -326,9 +309,6 @@
     </r>
   </si>
   <si>
-    <t>(0,15; 0,30; 0,25)%</t>
-  </si>
-  <si>
     <t>(1%; 6%) (0,25%; 5%)</t>
   </si>
   <si>
@@ -361,20 +341,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1,87 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 2,32</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">9,87 </t>
     </r>
     <r>
@@ -434,20 +400,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">9,7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 11,5</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">53,1 </t>
     </r>
     <r>
@@ -473,6 +425,192 @@
       </rPr>
       <t>± 0,057</t>
     </r>
+  </si>
+  <si>
+    <t>ATaF - humano</t>
+  </si>
+  <si>
+    <t>(8,515; 132,8)</t>
+  </si>
+  <si>
+    <t>(0,15; 0,30; 0,25)</t>
+  </si>
+  <si>
+    <t>(0,01; 0,001; 0,0001)</t>
+  </si>
+  <si>
+    <t>7,18 (N)</t>
+  </si>
+  <si>
+    <t>(0,092; 0,104; 0,144)</t>
+  </si>
+  <si>
+    <t>ATiF - humano</t>
+  </si>
+  <si>
+    <t>ATT - humano</t>
+  </si>
+  <si>
+    <t>CF - humano</t>
+  </si>
+  <si>
+    <t>PTaF - humano</t>
+  </si>
+  <si>
+    <t>PTiF - humano</t>
+  </si>
+  <si>
+    <t>PTT - humano</t>
+  </si>
+  <si>
+    <t>TiC - humano</t>
+  </si>
+  <si>
+    <t>(11,11; 217,1)</t>
+  </si>
+  <si>
+    <t>5,52 (N)</t>
+  </si>
+  <si>
+    <t>(0,091; 0,100; 0,158)</t>
+  </si>
+  <si>
+    <t>(6,95; 131,8)</t>
+  </si>
+  <si>
+    <t>2,06 (N)</t>
+  </si>
+  <si>
+    <t>(0,091; 0,084; 0,097)</t>
+  </si>
+  <si>
+    <t>(12,72; 244,1)</t>
+  </si>
+  <si>
+    <t>0,20 (N)</t>
+  </si>
+  <si>
+    <t>(0,069; 0,073; 0,209)</t>
+  </si>
+  <si>
+    <t>(9,48; 185;2)</t>
+  </si>
+  <si>
+    <t>0,14 (N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9,7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 11,5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">197,38 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 15,53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1,87 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 2,32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <t>0,001 (Mpa)</t>
+  </si>
+  <si>
+    <t>(0,078; 0,081; 0,146)</t>
+  </si>
+  <si>
+    <t>(12,86; 161,1)</t>
+  </si>
+  <si>
+    <t>6,87 (N)</t>
+  </si>
+  <si>
+    <t>(0,097; 0,112; 0,189)</t>
+  </si>
+  <si>
+    <t>(14,75; 216,9)</t>
+  </si>
+  <si>
+    <t>1,34 (N)</t>
+  </si>
+  <si>
+    <t>(0,127; 0,152; 0,284)</t>
+  </si>
+  <si>
+    <t>(11,16; 164,6)</t>
+  </si>
+  <si>
+    <t>0,51 (N)</t>
+  </si>
+  <si>
+    <t>(0,125; 0,152; 0,209)</t>
+  </si>
+  <si>
+    <t>(0,0032%; 5%)</t>
+  </si>
+  <si>
+    <t>(5%; 3,5%)</t>
   </si>
 </sst>
 </file>
@@ -944,7 +1082,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1202,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>14</v>
@@ -1217,65 +1355,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F196C40-960D-43DA-81EC-FA192A1581DD}">
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>40</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30">
-        <v>3.1999999999999999E-5</v>
-      </c>
-      <c r="C2" s="4"/>
+      <c r="B2" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.33</v>
+      </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="4">
-        <v>0.33</v>
-      </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1285,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1322,29 +1460,29 @@
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="27">
-        <v>0.05</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="4">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1352,7 +1490,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1368,16 +1506,16 @@
       <c r="B8" s="27">
         <v>0.05</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="F8" s="26">
+      <c r="D8" s="26">
         <v>2.78</v>
       </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1397,16 +1535,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -1427,18 +1565,18 @@
         <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="4">
+        <v>57</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D12" s="4">
+      <c r="F12" s="4">
         <v>199000</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H12" s="4">
         <v>161</v>
@@ -1452,26 +1590,26 @@
         <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="4">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1481,22 +1619,22 @@
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="J14" t="s">
         <v>64</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1506,22 +1644,22 @@
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="4">
+      <c r="C15" s="4">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="27">
         <v>0.05</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>10</v>
+      </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4">
-        <v>10</v>
-      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1529,14 +1667,14 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="4">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D17" s="4">
+      <c r="F17" s="4">
         <v>50</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4">
@@ -1545,21 +1683,21 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="29">
         <v>1E-3</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D18" s="4">
+      <c r="F18" s="4">
         <v>50</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4">
-        <v>1E-3</v>
+      <c r="G18" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="H18" s="4">
         <v>0.1</v>
@@ -1570,44 +1708,44 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="29">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="4">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4">
         <v>2.0649999999999999</v>
       </c>
-      <c r="D21" s="4">
+      <c r="F21" s="4">
         <v>2.2210000000000001</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1615,18 +1753,18 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1634,92 +1772,244 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="A23" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>180</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="4">
+        <v>12.5</v>
+      </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="A24" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="4">
+        <v>180</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.627</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="4">
+        <v>22.63</v>
+      </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="A25" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>180</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="4">
+        <v>20.11</v>
+      </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="A26" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>180</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="4">
+        <v>49.63</v>
+      </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="A27" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="4">
+        <v>180</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="4">
+        <v>44.35</v>
+      </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="A28" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C28" s="4">
+        <v>180</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="4">
+        <v>20.07</v>
+      </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="A29" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C29" s="4">
+        <v>180</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" s="4">
+        <v>28.65</v>
+      </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="A30" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="C30" s="4">
+        <v>180</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" s="4">
+        <v>45.99</v>
+      </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>

</xml_diff>

<commit_message>
Fixed all application to improve sensitivity analysis.
</commit_message>
<xml_diff>
--- a/sheets/númerosvisco.xlsx
+++ b/sheets/númerosvisco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\IC Tecidos Moles\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\SoftTissue\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBC80F2-21EB-4DEB-8A7B-57582F4DDA44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4BAFB1-14CE-4D44-A1EC-43EDB41D8E42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4560" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
+    <workbookView xWindow="0" yWindow="2295" windowWidth="27675" windowHeight="11385" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fized all application and added new solutions.
</commit_message>
<xml_diff>
--- a/sheets/númerosvisco.xlsx
+++ b/sheets/númerosvisco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\SoftTissue\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4BAFB1-14CE-4D44-A1EC-43EDB41D8E42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511BF9AA-1A07-4344-A2D5-0BB5E418439D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2295" windowWidth="27675" windowHeight="11385" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{F16226E8-CAA2-419C-ADF6-E1BB39C61BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="138">
   <si>
     <t>ACL - porco</t>
   </si>
@@ -368,8 +368,83 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">0,54 </t>
+    <t>(0,54; 1602)</t>
+  </si>
+  <si>
+    <t>ATaF - humano</t>
+  </si>
+  <si>
+    <t>(8,515; 132,8)</t>
+  </si>
+  <si>
+    <t>(0,15; 0,30; 0,25)</t>
+  </si>
+  <si>
+    <t>(0,01; 0,001; 0,0001)</t>
+  </si>
+  <si>
+    <t>7,18 (N)</t>
+  </si>
+  <si>
+    <t>(0,092; 0,104; 0,144)</t>
+  </si>
+  <si>
+    <t>ATiF - humano</t>
+  </si>
+  <si>
+    <t>ATT - humano</t>
+  </si>
+  <si>
+    <t>CF - humano</t>
+  </si>
+  <si>
+    <t>PTaF - humano</t>
+  </si>
+  <si>
+    <t>PTiF - humano</t>
+  </si>
+  <si>
+    <t>PTT - humano</t>
+  </si>
+  <si>
+    <t>(11,11; 217,1)</t>
+  </si>
+  <si>
+    <t>5,52 (N)</t>
+  </si>
+  <si>
+    <t>(0,091; 0,100; 0,158)</t>
+  </si>
+  <si>
+    <t>(6,95; 131,8)</t>
+  </si>
+  <si>
+    <t>2,06 (N)</t>
+  </si>
+  <si>
+    <t>(0,091; 0,084; 0,097)</t>
+  </si>
+  <si>
+    <t>(12,72; 244,1)</t>
+  </si>
+  <si>
+    <t>0,20 (N)</t>
+  </si>
+  <si>
+    <t>(0,069; 0,073; 0,209)</t>
+  </si>
+  <si>
+    <t>(9,48; 185;2)</t>
+  </si>
+  <si>
+    <t>0,14 (N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">197,38 </t>
     </r>
     <r>
       <rPr>
@@ -378,141 +453,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>± 0,15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1602 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 581</t>
-    </r>
-  </si>
-  <si>
-    <t>(0,54; 1602)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">53,1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0,089 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0,057</t>
-    </r>
-  </si>
-  <si>
-    <t>ATaF - humano</t>
-  </si>
-  <si>
-    <t>(8,515; 132,8)</t>
-  </si>
-  <si>
-    <t>(0,15; 0,30; 0,25)</t>
-  </si>
-  <si>
-    <t>(0,01; 0,001; 0,0001)</t>
-  </si>
-  <si>
-    <t>7,18 (N)</t>
-  </si>
-  <si>
-    <t>(0,092; 0,104; 0,144)</t>
-  </si>
-  <si>
-    <t>ATiF - humano</t>
-  </si>
-  <si>
-    <t>ATT - humano</t>
-  </si>
-  <si>
-    <t>CF - humano</t>
-  </si>
-  <si>
-    <t>PTaF - humano</t>
-  </si>
-  <si>
-    <t>PTiF - humano</t>
-  </si>
-  <si>
-    <t>PTT - humano</t>
-  </si>
-  <si>
-    <t>TiC - humano</t>
-  </si>
-  <si>
-    <t>(11,11; 217,1)</t>
-  </si>
-  <si>
-    <t>5,52 (N)</t>
-  </si>
-  <si>
-    <t>(0,091; 0,100; 0,158)</t>
-  </si>
-  <si>
-    <t>(6,95; 131,8)</t>
-  </si>
-  <si>
-    <t>2,06 (N)</t>
-  </si>
-  <si>
-    <t>(0,091; 0,084; 0,097)</t>
-  </si>
-  <si>
-    <t>(12,72; 244,1)</t>
-  </si>
-  <si>
-    <t>0,20 (N)</t>
-  </si>
-  <si>
-    <t>(0,069; 0,073; 0,209)</t>
-  </si>
-  <si>
-    <t>(9,48; 185;2)</t>
-  </si>
-  <si>
-    <t>0,14 (N)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">9,7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 11,5</t>
+      <t>± 15,53</t>
     </r>
     <r>
       <rPr>
@@ -527,7 +468,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">197,38 </t>
+      <t xml:space="preserve">1,87 </t>
     </r>
     <r>
       <rPr>
@@ -536,7 +477,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>± 15,53</t>
+      <t>± 2,32</t>
     </r>
     <r>
       <rPr>
@@ -550,8 +491,44 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1,87 </t>
+    <t>0,001 (Mpa)</t>
+  </si>
+  <si>
+    <t>(0,078; 0,081; 0,146)</t>
+  </si>
+  <si>
+    <t>(12,86; 161,1)</t>
+  </si>
+  <si>
+    <t>6,87 (N)</t>
+  </si>
+  <si>
+    <t>(0,097; 0,112; 0,189)</t>
+  </si>
+  <si>
+    <t>(14,75; 216,9)</t>
+  </si>
+  <si>
+    <t>1,34 (N)</t>
+  </si>
+  <si>
+    <t>(0,127; 0,152; 0,284)</t>
+  </si>
+  <si>
+    <t>(11,16; 164,6)</t>
+  </si>
+  <si>
+    <t>0,51 (N)</t>
+  </si>
+  <si>
+    <t>(0,125; 0,152; 0,209)</t>
+  </si>
+  <si>
+    <t>(0,0032%; 5%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(5%; 3,5%) (4,7 </t>
     </r>
     <r>
       <rPr>
@@ -560,7 +537,154 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>± 2,32</t>
+      <t>± 1,8)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(0,15) (0,26 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,01)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tecido Cerebral</t>
+  </si>
+  <si>
+    <t>(0,0051; 0, 051; 0,254)</t>
+  </si>
+  <si>
+    <t>ACL - bovino</t>
+  </si>
+  <si>
+    <t>LCL - bovino</t>
+  </si>
+  <si>
+    <t>MCL - bovino</t>
+  </si>
+  <si>
+    <t>PCL - bovino</t>
+  </si>
+  <si>
+    <t>PT- bovino</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1,23 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,50 (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3,25 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 5,50 (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1,38 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,42 (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2,34 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 3,57 (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1,26 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,61 (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">20,17 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 4,69</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">24,73 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 6,33</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">19,91 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±</t>
     </r>
     <r>
       <rPr>
@@ -570,47 +694,167 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (Mpa)</t>
-    </r>
-  </si>
-  <si>
-    <t>0,001 (Mpa)</t>
-  </si>
-  <si>
-    <t>(0,078; 0,081; 0,146)</t>
-  </si>
-  <si>
-    <t>(12,86; 161,1)</t>
-  </si>
-  <si>
-    <t>6,87 (N)</t>
-  </si>
-  <si>
-    <t>(0,097; 0,112; 0,189)</t>
-  </si>
-  <si>
-    <t>(14,75; 216,9)</t>
-  </si>
-  <si>
-    <t>1,34 (N)</t>
-  </si>
-  <si>
-    <t>(0,127; 0,152; 0,284)</t>
-  </si>
-  <si>
-    <t>(11,16; 164,6)</t>
-  </si>
-  <si>
-    <t>0,51 (N)</t>
-  </si>
-  <si>
-    <t>(0,125; 0,152; 0,209)</t>
-  </si>
-  <si>
-    <t>(0,0032%; 5%)</t>
-  </si>
-  <si>
-    <t>(5%; 3,5%)</t>
+      <t xml:space="preserve"> 10,90</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30,27 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 8,23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">26,65 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 12,21</t>
+    </r>
+  </si>
+  <si>
+    <t>TiC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(9,7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 11,5) (0,7 ± 0,6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  (6,18) (Mpa)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(53,1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) (54,1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 18,9) (70,15)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(0,089 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,057) (0,201 ± 0,106) (0,065)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(1602 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">± 581) (1269 ± </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>291) (300)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(0,54 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) (0,80 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,43) (0,622)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -620,7 +864,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,6 +877,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -685,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -749,14 +999,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1202,7 +1448,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>14</v>
@@ -1355,42 +1601,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F196C40-960D-43DA-81EC-FA192A1581DD}">
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>38</v>
@@ -1406,14 +1652,14 @@
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
         <v>0.33</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1460,29 +1706,29 @@
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1503,16 +1749,16 @@
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="26">
         <v>0.05</v>
       </c>
-      <c r="D8" s="26">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="F8" s="25">
         <v>2.78</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>43</v>
@@ -1537,14 +1783,14 @@
       <c r="B10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -1567,14 +1813,14 @@
       <c r="B12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
+      <c r="C12" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F12" s="4">
+      <c r="D12" s="4">
         <v>199000</v>
       </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
         <v>58</v>
       </c>
@@ -1592,18 +1838,18 @@
       <c r="B13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="4">
         <v>10</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>72</v>
@@ -1619,14 +1865,14 @@
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1638,43 +1884,43 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="4">
+      <c r="E15" s="4">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="26">
         <v>0.05</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
         <v>10</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4">
+      <c r="C17" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F17" s="4">
+      <c r="D17" s="4">
         <v>50</v>
       </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4">
@@ -1682,22 +1928,22 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="27">
         <v>1E-3</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4">
+      <c r="C18" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F18" s="4">
+      <c r="D18" s="4">
         <v>50</v>
       </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H18" s="4">
         <v>0.1</v>
@@ -1707,26 +1953,26 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="27">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1734,25 +1980,25 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4">
+      <c r="C21" s="4">
         <v>2.0649999999999999</v>
       </c>
-      <c r="F21" s="4">
+      <c r="D21" s="4">
         <v>2.2210000000000001</v>
       </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1760,11 +2006,11 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1772,250 +2018,259 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="4">
+        <v>180</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B23" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="C23" s="4">
-        <v>180</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0.55800000000000005</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="H23" s="4">
         <v>12.5</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="27">
+      <c r="A24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="26">
         <v>0.2</v>
       </c>
       <c r="C24" s="4">
+        <v>0.627</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="4">
         <v>180</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0.627</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H24" s="4">
         <v>22.63</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="27">
+      <c r="A25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="26">
         <v>0.2</v>
       </c>
       <c r="C25" s="4">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="4">
         <v>180</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0.46500000000000002</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H25" s="4">
         <v>20.11</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="27">
+      <c r="A26" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="26">
         <v>0.2</v>
       </c>
       <c r="C26" s="4">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="4">
         <v>180</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0.60499999999999998</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H26" s="4">
         <v>49.63</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="27">
+      <c r="A27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="26">
         <v>0.2</v>
       </c>
       <c r="C27" s="4">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="4">
         <v>180</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.47199999999999998</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4">
         <v>44.35</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="27">
+      <c r="A28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="26">
         <v>0.2</v>
       </c>
       <c r="C28" s="4">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="4">
         <v>180</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0.76500000000000001</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H28" s="4">
         <v>20.07</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="27">
+      <c r="A29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="26">
         <v>0.2</v>
       </c>
       <c r="C29" s="4">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="4">
         <v>180</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0.83199999999999996</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H29" s="4">
         <v>28.65</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="27">
+      <c r="A30" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="26">
         <v>0.2</v>
       </c>
       <c r="C30" s="4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="4">
         <v>180</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0.70399999999999996</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H30" s="4">
         <v>45.99</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="4">
+        <v>80</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2023,61 +2278,96 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2088,7 +2378,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2099,7 +2389,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -2110,7 +2400,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -2121,7 +2411,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2132,7 +2422,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2143,7 +2433,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2154,7 +2444,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2165,7 +2455,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2176,7 +2466,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2187,7 +2477,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2198,7 +2488,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -3849,6 +4139,7 @@
       <c r="J197" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>